<commit_message>
pulled hbil-dft and s66x8 MP2/aVQZ data for CP
</commit_message>
<xml_diff>
--- a/data/HBIL-dists_angles.xlsx
+++ b/data/HBIL-dists_angles.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26709"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,13 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="27960" yWindow="1020" windowWidth="20760" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="27200" yWindow="540" windowWidth="20760" windowHeight="17600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="61">
   <si>
     <t>DMEA-AcO-p1</t>
   </si>
@@ -99,14 +102,123 @@
   </si>
   <si>
     <t>EtMeNH2-mSO3-p1</t>
+  </si>
+  <si>
+    <t>EtNH3-AcO-p1</t>
+  </si>
+  <si>
+    <t>EtNH3-CF3SO3-p1</t>
+  </si>
+  <si>
+    <t>EtNH3-mSO3-p1</t>
+  </si>
+  <si>
+    <t>TMEA-AcO-p1</t>
+  </si>
+  <si>
+    <t>TMEA-CF3SO3-p1</t>
+  </si>
+  <si>
+    <t>TMEA-Cl-p1</t>
+  </si>
+  <si>
+    <t>TMEA-NO3-p1</t>
+  </si>
+  <si>
+    <t>TMEA-TFA-p1</t>
+  </si>
+  <si>
+    <t>TMEA-mOSO3-p1</t>
+  </si>
+  <si>
+    <t>TMEA-mSO3-p1</t>
+  </si>
+  <si>
+    <t>mim-AcO-p1</t>
+  </si>
+  <si>
+    <t>mim-CF3SO3-p1</t>
+  </si>
+  <si>
+    <t>mim-CF3SO3-p2</t>
+  </si>
+  <si>
+    <t>mim-Cl-p1</t>
+  </si>
+  <si>
+    <t>mim-Cl-p2</t>
+  </si>
+  <si>
+    <t>mim-NO3-p1</t>
+  </si>
+  <si>
+    <t>mim-NO3-p2</t>
+  </si>
+  <si>
+    <t>mim-TFA-p1</t>
+  </si>
+  <si>
+    <t>mim-TFA-p3</t>
+  </si>
+  <si>
+    <t>mim-mOSO3-p1</t>
+  </si>
+  <si>
+    <t>mim-mSO3-p1</t>
+  </si>
+  <si>
+    <t>mpyr-AcO-p1</t>
+  </si>
+  <si>
+    <t>mpyr-CF3SO3-p1</t>
+  </si>
+  <si>
+    <t>mpyr-Cl-p1</t>
+  </si>
+  <si>
+    <t>mpyr-NO3-p1</t>
+  </si>
+  <si>
+    <t>mpyr-TFA-p1</t>
+  </si>
+  <si>
+    <t>mpyr-mOSO3-p1</t>
+  </si>
+  <si>
+    <t>mpyr-mSO3-p1</t>
+  </si>
+  <si>
+    <t>mim-TFA-p2</t>
+  </si>
+  <si>
+    <t>mim-mSO3-p2</t>
+  </si>
+  <si>
+    <t>135.733/110.716 bond length/angle for other H-bond</t>
+  </si>
+  <si>
+    <t>EtNH3-Cl-p1</t>
+  </si>
+  <si>
+    <t>EtNH3-NO3-p1</t>
+  </si>
+  <si>
+    <t>EtNH3-TFA-p1</t>
+  </si>
+  <si>
+    <t>EtNH3-mOSO3-p1</t>
+  </si>
+  <si>
+    <t>1.80536/142.749 (NHO)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -137,9 +249,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,20 +530,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J15"/>
+  <dimension ref="B1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="2"/>
     <col min="4" max="4" width="10.83203125" style="1"/>
+    <col min="7" max="7" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -442,7 +557,7 @@
       <c r="F1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="J1" t="s">
@@ -453,7 +568,7 @@
       <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>1.03887</v>
       </c>
       <c r="D2" s="1">
@@ -465,7 +580,7 @@
       <c r="F2">
         <v>112.46899999999999</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="1">
         <v>-174.68899999999999</v>
       </c>
       <c r="H2" t="s">
@@ -479,7 +594,7 @@
       <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>1.7036500000000001</v>
       </c>
       <c r="D3" s="1">
@@ -488,7 +603,7 @@
       <c r="F3">
         <v>119.33199999999999</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="1">
         <v>-3.1539999999999999</v>
       </c>
       <c r="H3" t="s">
@@ -499,7 +614,7 @@
       <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>1.86608</v>
       </c>
       <c r="D4" s="1">
@@ -508,7 +623,7 @@
       <c r="F4" t="s">
         <v>6</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H4" t="s">
@@ -519,7 +634,7 @@
       <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>1.5466200000000001</v>
       </c>
       <c r="D5" s="1">
@@ -528,7 +643,7 @@
       <c r="F5">
         <v>105.788</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="1">
         <v>-179.35</v>
       </c>
       <c r="H5" t="s">
@@ -539,7 +654,7 @@
       <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>1.50038</v>
       </c>
       <c r="D6" s="1">
@@ -548,7 +663,7 @@
       <c r="F6">
         <v>106.526</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="1">
         <v>-30.808</v>
       </c>
       <c r="H6" t="s">
@@ -559,7 +674,7 @@
       <c r="B7" t="s">
         <v>10</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <v>1.6064000000000001</v>
       </c>
       <c r="D7" s="1">
@@ -568,7 +683,7 @@
       <c r="F7">
         <v>110.167</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="1">
         <v>-40.509</v>
       </c>
       <c r="H7" t="s">
@@ -579,7 +694,7 @@
       <c r="B8" t="s">
         <v>11</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="2">
         <v>1.5361100000000001</v>
       </c>
       <c r="D8" s="1">
@@ -588,7 +703,7 @@
       <c r="F8">
         <v>111.297</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="1">
         <v>22.309000000000001</v>
       </c>
       <c r="H8" t="s">
@@ -604,7 +719,7 @@
       <c r="B10" t="s">
         <v>19</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="2">
         <v>1.7688600000000001</v>
       </c>
       <c r="D10" s="1">
@@ -613,7 +728,7 @@
       <c r="F10">
         <v>103.093</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="1">
         <v>-26.86</v>
       </c>
       <c r="H10" t="s">
@@ -624,7 +739,7 @@
       <c r="B11" t="s">
         <v>20</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="2">
         <v>1.8917200000000001</v>
       </c>
       <c r="D11" s="1">
@@ -633,7 +748,7 @@
       <c r="F11" t="s">
         <v>6</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -641,7 +756,7 @@
       <c r="B12" t="s">
         <v>21</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="2">
         <v>1.5526500000000001</v>
       </c>
       <c r="D12" s="1">
@@ -650,7 +765,7 @@
       <c r="F12">
         <v>104.342</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="1">
         <v>-36.798999999999999</v>
       </c>
     </row>
@@ -658,7 +773,7 @@
       <c r="B13" t="s">
         <v>22</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="2">
         <v>1.52152</v>
       </c>
       <c r="D13" s="1">
@@ -667,7 +782,7 @@
       <c r="F13">
         <v>101.89700000000001</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="1">
         <v>-24.802</v>
       </c>
     </row>
@@ -675,7 +790,7 @@
       <c r="B14" t="s">
         <v>23</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="2">
         <v>1.7132499999999999</v>
       </c>
       <c r="D14" s="1">
@@ -684,7 +799,7 @@
       <c r="F14">
         <v>104.226</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="1">
         <v>-23.789000000000001</v>
       </c>
     </row>
@@ -692,7 +807,7 @@
       <c r="B15" t="s">
         <v>24</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="2">
         <v>1.7515799999999999</v>
       </c>
       <c r="D15" s="1">
@@ -701,8 +816,283 @@
       <c r="F15">
         <v>105.52200000000001</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="1">
         <v>-10.795999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="2">
+        <v>1.6373</v>
+      </c>
+      <c r="D16" s="1">
+        <v>163.11199999999999</v>
+      </c>
+      <c r="E16">
+        <v>1.6370199999999999</v>
+      </c>
+      <c r="F16">
+        <v>126.49</v>
+      </c>
+      <c r="G16" s="1">
+        <v>136.613</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="2">
+        <v>1.8427800000000001</v>
+      </c>
+      <c r="D17" s="1">
+        <v>144.761</v>
+      </c>
+      <c r="E17">
+        <v>1.9504999999999999</v>
+      </c>
+      <c r="F17">
+        <v>109.34399999999999</v>
+      </c>
+      <c r="G17" s="1">
+        <v>-16.667999999999999</v>
+      </c>
+      <c r="H17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="2">
+        <v>1.9028700000000001</v>
+      </c>
+      <c r="D18" s="1">
+        <v>169.20699999999999</v>
+      </c>
+      <c r="F18" t="s">
+        <v>6</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="2">
+        <v>1.54939</v>
+      </c>
+      <c r="D19" s="1">
+        <v>168.76400000000001</v>
+      </c>
+      <c r="F19">
+        <v>105.295</v>
+      </c>
+      <c r="G19" s="1">
+        <v>-33.479999999999997</v>
+      </c>
+      <c r="H19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" s="2">
+        <v>1.45394</v>
+      </c>
+      <c r="D20" s="1">
+        <v>166.97</v>
+      </c>
+      <c r="F20">
+        <v>102.895</v>
+      </c>
+      <c r="G20" s="1">
+        <v>23.524999999999999</v>
+      </c>
+      <c r="H20" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" s="2">
+        <v>1.66107</v>
+      </c>
+      <c r="D21" s="1">
+        <v>161.18</v>
+      </c>
+      <c r="F21">
+        <v>103.449</v>
+      </c>
+      <c r="G21" s="1">
+        <v>-29.39</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="2">
+        <v>1.80535</v>
+      </c>
+      <c r="D22" s="1">
+        <v>142.755</v>
+      </c>
+      <c r="F22">
+        <v>109.631</v>
+      </c>
+      <c r="G22" s="1">
+        <v>-21.157</v>
+      </c>
+      <c r="H22" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B46" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B48" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B49" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>